<commit_message>
Tracing fix and removed screenshot
</commit_message>
<xml_diff>
--- a/src/main/java/com/sample/testdata/ListOfItems.xlsx
+++ b/src/main/java/com/sample/testdata/ListOfItems.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/pavamshikrishna/eclipse-workspace/SampleProject/src/main/java/com/sample/testdata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B659439-408A-0049-9ACE-21D5A44DC853}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1CEBC55-B707-BC44-94A7-348A217EDBA0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16640" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -54,15 +54,6 @@
     <t>Result3</t>
   </si>
   <si>
-    <t>ifb washing machine</t>
-  </si>
-  <si>
-    <t>IFB</t>
-  </si>
-  <si>
-    <t>8 Kg</t>
-  </si>
-  <si>
     <t>5 Star</t>
   </si>
   <si>
@@ -75,7 +66,16 @@
     <t>128GB</t>
   </si>
   <si>
-    <t>Starlight</t>
+    <t>samsung 1.5 ton 5star</t>
+  </si>
+  <si>
+    <t>Samsung</t>
+  </si>
+  <si>
+    <t>1.5 Ton</t>
+  </si>
+  <si>
+    <t>Pink</t>
   </si>
 </sst>
 </file>
@@ -134,10 +134,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="1" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="1" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1"/>
@@ -426,51 +425,51 @@
   <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="43.33203125" style="6" customWidth="1"/>
+    <col min="1" max="1" width="43.33203125" style="5" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D2" t="s">
         <v>4</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="C2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D2" t="s">
-        <v>7</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A3" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="B3" s="3" t="s">
-        <v>9</v>
+      <c r="A3" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>6</v>
       </c>
       <c r="C3" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="D3" t="s">
         <v>11</v>

</xml_diff>